<commit_message>
upbit auto buy/sell ver.1
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -642,6 +642,176 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>13:55:38</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>이더리움클래식</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>110670.6658</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>082a421a-e786-4299-a80b-3e1073f8ea0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>13:55:38</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>이더리움클래식</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>110670.6658</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>082a421a-e786-4299-a80b-3e1073f8ea0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>13:55:38</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>이더리움클래식</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>110670.6658</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>082a421a-e786-4299-a80b-3e1073f8ea0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>13:55:38</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>이더리움클래식</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>110670.6658</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>082a421a-e786-4299-a80b-3e1073f8ea0e</t>
+        </is>
+      </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>1040</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>13:55:38</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>이더리움클래식</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>110670.6658</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>082a421a-e786-4299-a80b-3e1073f8ea0e</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>41160</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -653,7 +823,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -1250,19 +1420,259 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="n">
         <v>1135</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="0" t="n">
         <v>907.8</v>
       </c>
       <c r="D39" s="6" t="n">
-        <v>44601.57301973009</v>
+        <v>44601.5730197338</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>KRW-BORA</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1692.5</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1530</v>
+      </c>
+      <c r="D40" s="6" t="n">
+        <v>44601.57718226852</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>KRW-BORA</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1692.5</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1530</v>
+      </c>
+      <c r="D41" s="6" t="n">
+        <v>44601.5786025</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1135</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>907.8</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <v>44601.63494277777</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1135</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>907.8</v>
+      </c>
+      <c r="D43" s="6" t="n">
+        <v>44601.63601146991</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>KRW-ETH</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>3921500</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>3741800</v>
+      </c>
+      <c r="D44" s="6" t="n">
+        <v>44601.63768543981</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>KRW-ETH</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>3921500</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>3741800</v>
+      </c>
+      <c r="D45" s="6" t="n">
+        <v>44601.63831017361</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>13540</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="D46" s="6" t="n">
+        <v>44601.64621123843</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1135</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>907.8</v>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>44601.67166594908</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>KRW-ETC</t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>40880</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>37570</v>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>44601.67844353009</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>13540</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="D49" s="6" t="n">
+        <v>44601.68535065973</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>13540</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="D50" s="6" t="n">
+        <v>44601.68640888889</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>13540</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="D51" s="6" t="n">
+        <v>44601.68904278935</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>13540</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>12610</v>
+      </c>
+      <c r="D52" s="6" t="n">
+        <v>44601.69303079861</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WEMIX</t>
+        </is>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>8882.5</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>7750</v>
+      </c>
+      <c r="D53" s="6" t="n">
+        <v>44601.70851663194</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>KRW-WEMIX</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>10767.5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>8503</v>
+      </c>
+      <c r="D54" s="6" t="n">
+        <v>44601.73158772704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto upbit trade ver.0
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -812,6 +812,422 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>21:44:34</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>4.8534888</t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>444a70da-0365-4607-a66a-73cdd45a4e21</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>21:54:54</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>5212.2153</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>6ff17436-f504-4e7f-b09a-264a09bf94c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>07:06:22</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>4c3d3cec-56e9-4eb9-b9f9-4383a3007b4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>07:06:58</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>ba08ce51-cb08-431b-b5ef-e0bacff45b25</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>07:07:33</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>d8554c33-24fa-44d6-a94b-654648f993b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>07:07:35</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>76d4f85e-2a4d-4af8-b074-cb6b4346fae4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>07:07:36</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>f8681527-0c7a-40f1-ab31-37a46f547206</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>07:08:09</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>1ab51fbf-78d0-46af-b163-57aa7466d865</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>07:08:11</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>b0db772e-8f0d-4191-b84b-7f4467d782ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>07:08:12</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>f129d5d6-84b9-4287-862b-1b8c459e5492</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>07:08:48</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>397023da-cbc6-445b-a575-44d8fe385c19</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>07:09:25</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>184b5087-0041-45cc-bd75-3d302b749511</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>07:09:26</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>10000.0</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>d545f2f0-2389-4109-a313-97e5fef2fff9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -823,7 +1239,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -1660,19 +2076,259 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="0" t="inlineStr">
         <is>
           <t>KRW-WEMIX</t>
         </is>
       </c>
-      <c r="B54" t="n">
+      <c r="B54" s="0" t="n">
         <v>10767.5</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" s="0" t="n">
         <v>8503</v>
       </c>
       <c r="D54" s="6" t="n">
-        <v>44601.73158772704</v>
+        <v>44601.73158773148</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WEMIX</t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>10767.5</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>8503</v>
+      </c>
+      <c r="D55" s="6" t="n">
+        <v>44601.73961967593</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WEMIX</t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>9447.5</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>8652</v>
+      </c>
+      <c r="D56" s="6" t="n">
+        <v>44601.77413966435</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>9840</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>8943</v>
+      </c>
+      <c r="D57" s="6" t="n">
+        <v>44601.89916591435</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1047.5</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>1039</v>
+      </c>
+      <c r="D58" s="6" t="n">
+        <v>44601.91312703703</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D59" s="6" t="n">
+        <v>44602.29608865741</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D60" s="6" t="n">
+        <v>44602.29650474537</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>1078</v>
+      </c>
+      <c r="D61" s="6" t="n">
+        <v>44602.29691423611</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D62" s="6" t="n">
+        <v>44602.29693200231</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>5765</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>5716</v>
+      </c>
+      <c r="D63" s="6" t="n">
+        <v>44602.29694398148</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>1078</v>
+      </c>
+      <c r="D64" s="6" t="n">
+        <v>44602.29733469908</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D65" s="6" t="n">
+        <v>44602.29735072917</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>5765</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>5716</v>
+      </c>
+      <c r="D66" s="6" t="n">
+        <v>44602.29736428241</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D67" s="6" t="n">
+        <v>44602.29778336806</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>14390</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>14234</v>
+      </c>
+      <c r="D68" s="6" t="n">
+        <v>44602.2982105787</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>KRW-SAND</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>5765</v>
+      </c>
+      <c r="C69" t="n">
+        <v>5716</v>
+      </c>
+      <c r="D69" s="6" t="n">
+        <v>44602.29822403163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto upbit trade ver.0.1
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1228,6 +1228,70 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-12</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>21:46:56</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>KRW-STRK</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>10731.0</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>e2e09f78-b451-4430-af97-abef1dd5b7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2022-02-13</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>09:04:22</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>KRW-STRK</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.48524233</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>88d9f1b0-be10-4cb2-aa72-fa3eeb406b2d</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1239,7 +1303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -2316,19 +2380,38 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="0" t="inlineStr">
         <is>
           <t>KRW-SAND</t>
         </is>
       </c>
-      <c r="B69" t="n">
+      <c r="B69" s="0" t="n">
         <v>5765</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" s="0" t="n">
         <v>5716</v>
       </c>
       <c r="D69" s="6" t="n">
-        <v>44602.29822403163</v>
+        <v>44602.29822402778</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
+        <is>
+          <t>KRW-STRK</t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>44810</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>44758</v>
+      </c>
+      <c r="D70" s="6" t="n">
+        <v>44604.90759403935</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>10731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upbit auto trade ver.2.2
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1870,6 +1870,230 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>17:39:36</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>10627.0</t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>9c68a327-011f-40c7-aaab-7fb3e6a82e24</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>17:53:00</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>10622.0</t>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t>3ec23625-253e-4bd9-b121-c553c77e79bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>17:55:37</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>10620.0</t>
+        </is>
+      </c>
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t>14c6b3c8-7d34-451c-a15a-8ed956e43efb</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>18:00:08</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
+        <is>
+          <t>10616.0</t>
+        </is>
+      </c>
+      <c r="F47" s="0" t="inlineStr">
+        <is>
+          <t>76bf3d98-ba17-4ff7-8d9f-04374860f020</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>18:18:03</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>10612.0</t>
+        </is>
+      </c>
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t>aad39f65-ab99-4622-ae22-ab2a8973cc35</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>21:45:42</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
+        <is>
+          <t>11.06569343</t>
+        </is>
+      </c>
+      <c r="F49" s="0" t="inlineStr">
+        <is>
+          <t>57369706-ab8a-4304-bcde-a3509bb94f63</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>21:45:45</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E50" s="0" t="inlineStr">
+        <is>
+          <t>10626.0</t>
+        </is>
+      </c>
+      <c r="F50" s="0" t="inlineStr">
+        <is>
+          <t>3489bed7-7dae-4a51-bff0-8a3b4f842c7b</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1881,7 +2105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -3296,6 +3520,120 @@
         <v>10632</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D87" s="7" t="n">
+        <v>44606.73583745371</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>10627</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D88" s="7" t="n">
+        <v>44606.74513364583</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>10622</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D89" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>10620</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D90" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>10616</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D91" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>10612</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>1017.5</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>996.4</v>
+      </c>
+      <c r="D92" s="7" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>10626</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3307,7 +3645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A120" sqref="A120"/>
@@ -3353,234 +3691,1066 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>f553fb4e-614d-4dcd-b3be-3ca7a8c9c19e</t>
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>969</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>cef7c6f3-7440-4d71-9978-758c9431264c</t>
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>959</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>43315dc0-2a7a-4b19-b4fd-c370a529a888</t>
         </is>
       </c>
       <c r="B4" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>949</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>525d3676-4ab7-4c80-9c2c-ce09f6014136</t>
         </is>
       </c>
       <c r="B5" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>939</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>89f153b2-9a89-4b6d-ab1e-d5e292367119</t>
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>929</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>960ee5e0-75fb-44c5-9be6-457494a736ae</t>
         </is>
       </c>
       <c r="B7" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>919</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>9b1917c0-18dd-4519-8ae8-3794ec6c7ecf</t>
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>909</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>ec2b0e9f-ff19-4ef9-a71a-29932fa4a750</t>
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>899</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>d43bfe99-995d-4eed-a3dc-75c38a253587</t>
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>44606.71858867691</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+        <v>44606.71858868055</v>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>889</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="0" t="n">
         <v>10.86006129</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>5f673a41-10ef-4150-abc3-89de1a1558e0</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>954</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>11.13207547</v>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>cd64496b-1603-47de-9320-046220dc17c5</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>944</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>11.25</v>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>77f3b3c1-2353-4e00-a524-f6300d079d09</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>934</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>11.37044968</v>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>3980c2c4-14f5-40c8-94f2-6a11b76f4293</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>924</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>11.49350649</v>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>8cac5837-a8d5-43f4-99e0-49d37d7e45ad</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>914</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>11.61925602</v>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>57b9dd92-de85-481c-a404-4b4a1d395402</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>904</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>11.74778761</v>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>fb729d80-1c8f-476b-b06c-bd471334787e</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>894</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>11.87919463</v>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>bb3d5e05-052e-4b18-a56a-d23cd0d752d6</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>44606.74695302083</v>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>884</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>12.01357466</v>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>c6634c1c-6ce6-4387-987f-b29d3fcbb9fa</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>951</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>11.16298633</v>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>76b8c985-17f6-41cf-a214-8ece4905cac0</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>941</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>11.2816153</v>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>84cdb964-a28b-4199-95ae-bcb473b33625</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>931</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>11.4027927</v>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>5526f364-7ec4-4b67-9b5f-916c535e7a79</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>921</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>11.52660152</v>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>22f101a6-48c6-47ab-ad65-a8f49aec66a0</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>911</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>11.65312843</v>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>8fa36280-55fc-4574-9bf7-78cfdf41f6dd</t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>901</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>11.78246393</v>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>0ddf733e-cd6a-40fc-ac22-7b7e8635ceb2</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>891</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>11.91470258</v>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>2d2ffca8-42ca-4436-b14d-90b67b69d667</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="n">
+        <v>44606.75009982639</v>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>881</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>12.04994325</v>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>af6f754f-d82b-4326-99d1-336171ead12e</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>949</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>11.18229715</v>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>b794ad80-9cc1-41bb-8d7a-f1830c011d8b</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>939</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>11.30138445</v>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>ef67044a-52d5-4200-a18a-b38e1207a5e8</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>929</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>11.42303552</v>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>2ddb74b3-21ed-48bf-939e-a55f5afdc5a3</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>919</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>11.54733406</v>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>4eeba694-b6e2-4c28-b00c-574394f61fa0</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>909</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>11.67436744</v>
+      </c>
+      <c r="F31" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>d3d71dc4-52b6-4cbe-b1c1-ad008659e9cf</t>
+        </is>
+      </c>
+      <c r="B32" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>11.80422692</v>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>d942da04-1e6c-4126-a50e-af5568642412</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>889</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>11.93700787</v>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>84d24548-83b8-4490-9056-7da682f89848</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>44606.76253762731</v>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>879</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>12.07281001</v>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>8c092722-bcbb-4ec8-8875-a747e5562788</t>
+        </is>
+      </c>
+      <c r="B35" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>964</v>
+      </c>
+      <c r="E35" t="n">
+        <v>11.02282158</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ea9dbef9-816b-41e1-ba64-0dc8e4a7d538</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>954</v>
+      </c>
+      <c r="E36" t="n">
+        <v>11.13836478</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>3b6071a7-bd42-435c-9156-f30f6a4e5e7a</t>
+        </is>
+      </c>
+      <c r="B37" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>944</v>
+      </c>
+      <c r="E37" t="n">
+        <v>11.25635593</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>f90b2e0f-3190-48e3-8682-a76f53ba65f4</t>
+        </is>
+      </c>
+      <c r="B38" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>934</v>
+      </c>
+      <c r="E38" t="n">
+        <v>11.37687366</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2fd25e05-8c8e-4eb8-bfe1-f60063cb9518</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>924</v>
+      </c>
+      <c r="E39" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>059556c0-fd1d-450d-9e5e-b0bf6ee5f66f</t>
+        </is>
+      </c>
+      <c r="B40" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>914</v>
+      </c>
+      <c r="E40" t="n">
+        <v>11.62582057</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>a17f984b-3214-4c88-bd19-446ae82bc9ce</t>
+        </is>
+      </c>
+      <c r="B41" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>904</v>
+      </c>
+      <c r="E41" t="n">
+        <v>11.75442478</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>fe66ac79-57ab-440f-a792-a64a9c68bb35</t>
+        </is>
+      </c>
+      <c r="B42" s="7" t="n">
+        <v>44606.90676508552</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>894</v>
+      </c>
+      <c r="E42" t="n">
+        <v>11.88590604</v>
+      </c>
+      <c r="F42" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>

</xml_diff>

<commit_message>
upbit auto trade v.2.2
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -473,13 +473,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col width="37.28515625" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
   </cols>
@@ -2091,6 +2091,70 @@
       <c r="F50" s="0" t="inlineStr">
         <is>
           <t>3489bed7-7dae-4a51-bff0-8a3b4f842c7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-15</t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>10:21:59</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E51" s="0" t="inlineStr">
+        <is>
+          <t>11.67606225</t>
+        </is>
+      </c>
+      <c r="F51" s="0" t="inlineStr">
+        <is>
+          <t>9cd6b065-59c6-4079-9d01-6552963a6f63</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>2022-02-15</t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>23:52:01</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
+        <is>
+          <t>KRW-BTC</t>
+        </is>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E52" s="0" t="inlineStr">
+        <is>
+          <t>10604.0</t>
+        </is>
+      </c>
+      <c r="F52" s="0" t="inlineStr">
+        <is>
+          <t>62f5a1a6-e346-47a6-bf80-a5850eec89c5</t>
         </is>
       </c>
     </row>
@@ -2105,13 +2169,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col width="11.7109375" bestFit="1" customWidth="1" style="3" min="2" max="3"/>
     <col width="19.140625" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
@@ -3632,6 +3696,25 @@
       </c>
       <c r="E92" s="0" t="n">
         <v>10626</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>KRW-BTC</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>52234500</v>
+      </c>
+      <c r="C93" t="n">
+        <v>51947600</v>
+      </c>
+      <c r="D93" s="7" t="n">
+        <v>44607.99442908435</v>
+      </c>
+      <c r="E93" t="n">
+        <v>10604</v>
       </c>
     </row>
   </sheetData>
@@ -3651,7 +3734,7 @@
       <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col width="37.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.5703125" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
@@ -4549,208 +4632,208 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="0" t="inlineStr">
         <is>
           <t>8c092722-bcbb-4ec8-8875-a747e5562788</t>
         </is>
       </c>
       <c r="B35" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="n">
         <v>964</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" s="0" t="n">
         <v>11.02282158</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>ea9dbef9-816b-41e1-ba64-0dc8e4a7d538</t>
         </is>
       </c>
       <c r="B36" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="n">
         <v>954</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" s="0" t="n">
         <v>11.13836478</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>3b6071a7-bd42-435c-9156-f30f6a4e5e7a</t>
         </is>
       </c>
       <c r="B37" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="n">
         <v>944</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" s="0" t="n">
         <v>11.25635593</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>f90b2e0f-3190-48e3-8682-a76f53ba65f4</t>
         </is>
       </c>
       <c r="B38" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="n">
         <v>934</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" s="0" t="n">
         <v>11.37687366</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="0" t="inlineStr">
         <is>
           <t>2fd25e05-8c8e-4eb8-bfe1-f60063cb9518</t>
         </is>
       </c>
       <c r="B39" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>924</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" s="0" t="n">
         <v>11.5</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="0" t="inlineStr">
         <is>
           <t>059556c0-fd1d-450d-9e5e-b0bf6ee5f66f</t>
         </is>
       </c>
       <c r="B40" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="n">
         <v>914</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" s="0" t="n">
         <v>11.62582057</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="0" t="inlineStr">
         <is>
           <t>a17f984b-3214-4c88-bd19-446ae82bc9ce</t>
         </is>
       </c>
       <c r="B41" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="n">
         <v>904</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" s="0" t="n">
         <v>11.75442478</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="0" t="inlineStr">
         <is>
           <t>fe66ac79-57ab-440f-a792-a64a9c68bb35</t>
         </is>
       </c>
       <c r="B42" s="7" t="n">
-        <v>44606.90676508552</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>KRW-XRP</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
+        <v>44606.90676508102</v>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="n">
         <v>894</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" s="0" t="n">
         <v>11.88590604</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" s="0" t="inlineStr">
         <is>
           <t>거미줄매수</t>
         </is>

</xml_diff>

<commit_message>
upbit auto trade v.3.0
</commit_message>
<xml_diff>
--- a/upbitRecord.xlsx
+++ b/upbitRecord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1360" yWindow="1320" windowWidth="27900" windowHeight="16820" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1360" yWindow="1320" windowWidth="27900" windowHeight="16820" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -510,16 +510,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G57" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F71" sqref="F71:F82"/>
+      <selection pane="bottomRight" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
   <cols>
     <col width="17" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="37.28515625" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
@@ -3663,6 +3663,1126 @@
       </c>
       <c r="G95" s="4" t="n">
         <v>1017606.7580248</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-29</t>
+        </is>
+      </c>
+      <c r="B96" s="4" t="inlineStr">
+        <is>
+          <t>20:04:16</t>
+        </is>
+      </c>
+      <c r="C96" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D96" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E96" s="4" t="inlineStr">
+        <is>
+          <t>100592.51</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>2e62e7b7-5ee6-458a-9d5c-084aa1a67f6e</t>
+        </is>
+      </c>
+      <c r="G96" s="4" t="n">
+        <v>1010986.29909927</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-29</t>
+        </is>
+      </c>
+      <c r="B97" s="4" t="inlineStr">
+        <is>
+          <t>20:08:06</t>
+        </is>
+      </c>
+      <c r="C97" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E97" s="4" t="inlineStr">
+        <is>
+          <t>100534.8</t>
+        </is>
+      </c>
+      <c r="F97" s="4" t="inlineStr">
+        <is>
+          <t>6f2bf445-0c30-4253-8086-aeb6ce1b3754</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="n">
+        <v>1010409.2032066</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-29</t>
+        </is>
+      </c>
+      <c r="B98" s="4" t="inlineStr">
+        <is>
+          <t>20:12:46</t>
+        </is>
+      </c>
+      <c r="C98" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D98" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E98" s="4" t="inlineStr">
+        <is>
+          <t>99973.17</t>
+        </is>
+      </c>
+      <c r="F98" s="4" t="inlineStr">
+        <is>
+          <t>94a37776-fa4b-49bb-8a5f-6196d7e0a454</t>
+        </is>
+      </c>
+      <c r="G98" s="4" t="n">
+        <v>1009832.43839433</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-29</t>
+        </is>
+      </c>
+      <c r="B99" s="4" t="inlineStr">
+        <is>
+          <t>20:16:44</t>
+        </is>
+      </c>
+      <c r="C99" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D99" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E99" s="4" t="inlineStr">
+        <is>
+          <t>100407.44</t>
+        </is>
+      </c>
+      <c r="F99" s="4" t="inlineStr">
+        <is>
+          <t>52a42613-0614-415e-9b3d-72228d30cc85</t>
+        </is>
+      </c>
+      <c r="G99" s="4" t="n">
+        <v>1009127.34035862</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="B100" s="4" t="inlineStr">
+        <is>
+          <t>01:12:26</t>
+        </is>
+      </c>
+      <c r="C100" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D100" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E100" s="4" t="inlineStr">
+        <is>
+          <t>3.31805295</t>
+        </is>
+      </c>
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>54270fb7-7b1b-4cd8-8faa-263c473f42cd</t>
+        </is>
+      </c>
+      <c r="G100" s="4" t="n">
+        <v>4350.08883634</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="B101" s="4" t="inlineStr">
+        <is>
+          <t>01:17:53</t>
+        </is>
+      </c>
+      <c r="C101" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D101" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E101" s="4" t="inlineStr">
+        <is>
+          <t>100897.975</t>
+        </is>
+      </c>
+      <c r="F101" s="4" t="inlineStr">
+        <is>
+          <t>d40fda7b-0c1c-41a9-9c9a-3d61ed1f5b8a</t>
+        </is>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>1014058.79312318</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="B102" s="4" t="inlineStr">
+        <is>
+          <t>07:34:59</t>
+        </is>
+      </c>
+      <c r="C102" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="D102" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E102" s="4" t="inlineStr">
+        <is>
+          <t>1.74061428</t>
+        </is>
+      </c>
+      <c r="F102" s="4" t="inlineStr">
+        <is>
+          <t>ef515d0a-70c6-4846-a716-bac28a5c01f5</t>
+        </is>
+      </c>
+      <c r="G102" s="4" t="n">
+        <v>4473.65472919</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="4" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="B103" s="4" t="inlineStr">
+        <is>
+          <t>07:40:31</t>
+        </is>
+      </c>
+      <c r="C103" s="4" t="inlineStr">
+        <is>
+          <t>KRW-BTC</t>
+        </is>
+      </c>
+      <c r="D103" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E103" s="4" t="inlineStr">
+        <is>
+          <t>101501.94</t>
+        </is>
+      </c>
+      <c r="F103" s="4" t="inlineStr">
+        <is>
+          <t>3f90f0e5-c0a4-49f4-8591-cc95fad9311b</t>
+        </is>
+      </c>
+      <c r="G103" s="4" t="n">
+        <v>1020128.99385442</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B104" s="4" t="inlineStr">
+        <is>
+          <t>00:01:56</t>
+        </is>
+      </c>
+      <c r="C104" s="4" t="inlineStr">
+        <is>
+          <t>KRW-BTC</t>
+        </is>
+      </c>
+      <c r="D104" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E104" s="4" t="inlineStr">
+        <is>
+          <t>0.00363356</t>
+        </is>
+      </c>
+      <c r="F104" s="4" t="inlineStr">
+        <is>
+          <t>951c3208-155c-4608-805a-386beb8a4895</t>
+        </is>
+      </c>
+      <c r="G104" s="4" t="n">
+        <v>4602.765655</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B105" s="4" t="inlineStr">
+        <is>
+          <t>00:04:50</t>
+        </is>
+      </c>
+      <c r="C105" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="D105" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E105" s="4" t="inlineStr">
+        <is>
+          <t>101687.01</t>
+        </is>
+      </c>
+      <c r="F105" s="4" t="inlineStr">
+        <is>
+          <t>46ee5517-13d1-448c-97dd-5ea06ccbc7b0</t>
+        </is>
+      </c>
+      <c r="G105" s="4" t="n">
+        <v>1021988.67862877</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B106" s="4" t="inlineStr">
+        <is>
+          <t>01:19:08</t>
+        </is>
+      </c>
+      <c r="C106" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="D106" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E106" s="4" t="inlineStr">
+        <is>
+          <t>0.62866775</t>
+        </is>
+      </c>
+      <c r="F106" s="4" t="inlineStr">
+        <is>
+          <t>47d26d2f-35b1-45de-a1ff-5197d4005aa4</t>
+        </is>
+      </c>
+      <c r="G106" s="4" t="n">
+        <v>4610.14755375</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B107" s="4" t="inlineStr">
+        <is>
+          <t>01:19:49</t>
+        </is>
+      </c>
+      <c r="C107" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ETH</t>
+        </is>
+      </c>
+      <c r="D107" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E107" s="4" t="inlineStr">
+        <is>
+          <t>101783.525</t>
+        </is>
+      </c>
+      <c r="F107" s="4" t="inlineStr">
+        <is>
+          <t>ea8967b4-e47a-4425-9859-7bdf87593d2b</t>
+        </is>
+      </c>
+      <c r="G107" s="4" t="n">
+        <v>1022955.19242762</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B108" s="4" t="inlineStr">
+        <is>
+          <t>03:05:05</t>
+        </is>
+      </c>
+      <c r="C108" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ETH</t>
+        </is>
+      </c>
+      <c r="D108" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E108" s="4" t="inlineStr">
+        <is>
+          <t>0.02438512</t>
+        </is>
+      </c>
+      <c r="F108" s="4" t="inlineStr">
+        <is>
+          <t>559baf34-a528-4e27-b0d5-10bb66bb4b63</t>
+        </is>
+      </c>
+      <c r="G108" s="4" t="n">
+        <v>4611.06035038</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B109" s="4" t="inlineStr">
+        <is>
+          <t>03:05:47</t>
+        </is>
+      </c>
+      <c r="C109" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="D109" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E109" s="4" t="inlineStr">
+        <is>
+          <t>101875.065</t>
+        </is>
+      </c>
+      <c r="F109" s="4" t="inlineStr">
+        <is>
+          <t>aa49267c-8bdd-4524-9bfb-f19001cbedd1</t>
+        </is>
+      </c>
+      <c r="G109" s="4" t="n">
+        <v>1023877.07188922</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B110" s="4" t="inlineStr">
+        <is>
+          <t>09:12:15</t>
+        </is>
+      </c>
+      <c r="C110" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="D110" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E110" s="4" t="inlineStr">
+        <is>
+          <t>0.62081087</t>
+        </is>
+      </c>
+      <c r="F110" s="4" t="inlineStr">
+        <is>
+          <t>3c7f10d1-eb8f-4d74-a094-2c01c7182437</t>
+        </is>
+      </c>
+      <c r="G110" s="4" t="n">
+        <v>921951.0705903301</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B111" s="4" t="inlineStr">
+        <is>
+          <t>09:12:52</t>
+        </is>
+      </c>
+      <c r="C111" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ZIL</t>
+        </is>
+      </c>
+      <c r="D111" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E111" s="4" t="inlineStr">
+        <is>
+          <t>101954.665</t>
+        </is>
+      </c>
+      <c r="F111" s="4" t="inlineStr">
+        <is>
+          <t>fd078a3d-31a1-4dfa-9d3c-60566d8f51fd</t>
+        </is>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>1024674.92249907</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B112" s="4" t="inlineStr">
+        <is>
+          <t>09:33:03</t>
+        </is>
+      </c>
+      <c r="C112" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ZIL</t>
+        </is>
+      </c>
+      <c r="D112" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E112" s="4" t="inlineStr">
+        <is>
+          <t>900.47695934</t>
+        </is>
+      </c>
+      <c r="F112" s="4" t="inlineStr">
+        <is>
+          <t>7e09f3d9-87c8-4361-aca0-1f6907cea42f</t>
+        </is>
+      </c>
+      <c r="G112" s="4" t="n">
+        <v>4618.49917544</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B113" s="4" t="inlineStr">
+        <is>
+          <t>09:33:50</t>
+        </is>
+      </c>
+      <c r="C113" s="4" t="inlineStr">
+        <is>
+          <t>KRW-AXS</t>
+        </is>
+      </c>
+      <c r="D113" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E113" s="4" t="inlineStr">
+        <is>
+          <t>102073.0699</t>
+        </is>
+      </c>
+      <c r="F113" s="4" t="inlineStr">
+        <is>
+          <t>eb17cbdc-16de-426d-8294-6285b8a98ba5</t>
+        </is>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>1025869.73019221</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B114" s="4" t="inlineStr">
+        <is>
+          <t>10:17:51</t>
+        </is>
+      </c>
+      <c r="C114" s="4" t="inlineStr">
+        <is>
+          <t>KRW-AXS</t>
+        </is>
+      </c>
+      <c r="D114" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E114" s="4" t="inlineStr">
+        <is>
+          <t>2.34020581</t>
+        </is>
+      </c>
+      <c r="F114" s="4" t="inlineStr">
+        <is>
+          <t>5aea306a-6cdd-4caf-a3ad-10b02d21f0b3</t>
+        </is>
+      </c>
+      <c r="G114" s="4" t="n">
+        <v>4628.66653796</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B115" s="4" t="inlineStr">
+        <is>
+          <t>10:20:03</t>
+        </is>
+      </c>
+      <c r="C115" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="D115" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E115" s="4" t="inlineStr">
+        <is>
+          <t>102280.03</t>
+        </is>
+      </c>
+      <c r="F115" s="4" t="inlineStr">
+        <is>
+          <t>c5727487-b5f0-4e8a-a696-9c229cbc0565</t>
+        </is>
+      </c>
+      <c r="G115" s="4" t="n">
+        <v>1027947.85749579</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B116" s="4" t="inlineStr">
+        <is>
+          <t>17:13:49</t>
+        </is>
+      </c>
+      <c r="C116" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="D116" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E116" s="4" t="inlineStr">
+        <is>
+          <t>11.45353079</t>
+        </is>
+      </c>
+      <c r="F116" s="4" t="inlineStr">
+        <is>
+          <t>f48522ac-9926-4d17-b88c-75ddb38eae0b</t>
+        </is>
+      </c>
+      <c r="G116" s="4" t="n">
+        <v>4636.15746165</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B117" s="4" t="inlineStr">
+        <is>
+          <t>17:14:28</t>
+        </is>
+      </c>
+      <c r="C117" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D117" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E117" s="4" t="inlineStr">
+        <is>
+          <t>102389.48</t>
+        </is>
+      </c>
+      <c r="F117" s="4" t="inlineStr">
+        <is>
+          <t>db313432-b2c0-46c5-ba44-87f06c1af05b</t>
+        </is>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>1029047.59688842</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B118" s="4" t="inlineStr">
+        <is>
+          <t>17:15:07</t>
+        </is>
+      </c>
+      <c r="C118" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D118" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E118" s="4" t="inlineStr">
+        <is>
+          <t>1294.43084702</t>
+        </is>
+      </c>
+      <c r="F118" s="4" t="inlineStr">
+        <is>
+          <t>4b8742a3-239c-4998-9d08-415f14867eeb</t>
+        </is>
+      </c>
+      <c r="G118" s="4" t="n">
+        <v>4640.84948919</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B119" s="4" t="inlineStr">
+        <is>
+          <t>17:15:46</t>
+        </is>
+      </c>
+      <c r="C119" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D119" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E119" s="4" t="inlineStr">
+        <is>
+          <t>102494.95</t>
+        </is>
+      </c>
+      <c r="F119" s="4" t="inlineStr">
+        <is>
+          <t>bb33650f-f825-4d60-b237-4746b748f7e4</t>
+        </is>
+      </c>
+      <c r="G119" s="4" t="n">
+        <v>1030109.61267686</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B120" s="4" t="inlineStr">
+        <is>
+          <t>17:17:59</t>
+        </is>
+      </c>
+      <c r="C120" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D120" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E120" s="4" t="inlineStr">
+        <is>
+          <t>1276.40037359</t>
+        </is>
+      </c>
+      <c r="F120" s="4" t="inlineStr">
+        <is>
+          <t>8a498663-ba50-41ad-9b7b-0718a780870a</t>
+        </is>
+      </c>
+      <c r="G120" s="4" t="n">
+        <v>4647.63792755</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B121" s="4" t="inlineStr">
+        <is>
+          <t>17:18:37</t>
+        </is>
+      </c>
+      <c r="C121" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D121" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E121" s="4" t="inlineStr">
+        <is>
+          <t>102625.295</t>
+        </is>
+      </c>
+      <c r="F121" s="4" t="inlineStr">
+        <is>
+          <t>18d28a1a-dd2e-40f8-86f7-96fcbea19ce9</t>
+        </is>
+      </c>
+      <c r="G121" s="4" t="n">
+        <v>1031410.4561176</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B122" s="4" t="inlineStr">
+        <is>
+          <t>17:23:39</t>
+        </is>
+      </c>
+      <c r="C122" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="D122" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E122" s="4" t="inlineStr">
+        <is>
+          <t>1265.41670776</t>
+        </is>
+      </c>
+      <c r="F122" s="4" t="inlineStr">
+        <is>
+          <t>3892e605-0abe-4b5d-87c7-781c30e29ac8</t>
+        </is>
+      </c>
+      <c r="G122" s="4" t="n">
+        <v>4644.37964359</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B123" s="4" t="inlineStr">
+        <is>
+          <t>17:24:21</t>
+        </is>
+      </c>
+      <c r="C123" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="D123" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E123" s="4" t="inlineStr">
+        <is>
+          <t>102702.905</t>
+        </is>
+      </c>
+      <c r="F123" s="4" t="inlineStr">
+        <is>
+          <t>33f2d874-1ee2-420a-b784-26416d6dc64e</t>
+        </is>
+      </c>
+      <c r="G123" s="4" t="n">
+        <v>1032193.17962218</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B124" s="4" t="inlineStr">
+        <is>
+          <t>19:14:07</t>
+        </is>
+      </c>
+      <c r="C124" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="D124" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E124" s="4" t="inlineStr">
+        <is>
+          <t>11.34838729</t>
+        </is>
+      </c>
+      <c r="F124" s="4" t="inlineStr">
+        <is>
+          <t>38e7911a-ebfd-413e-a769-2491c66178e5</t>
+        </is>
+      </c>
+      <c r="G124" s="4" t="n">
+        <v>4650.61517923</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B125" s="4" t="inlineStr">
+        <is>
+          <t>19:20:33</t>
+        </is>
+      </c>
+      <c r="C125" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SRM</t>
+        </is>
+      </c>
+      <c r="D125" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E125" s="4" t="inlineStr">
+        <is>
+          <t>102794.4449</t>
+        </is>
+      </c>
+      <c r="F125" s="4" t="inlineStr">
+        <is>
+          <t>00ec8b6f-46e0-4c3f-b8ed-6b159297b926</t>
+        </is>
+      </c>
+      <c r="G125" s="4" t="n">
+        <v>1033111.32089588</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B126" s="4" t="inlineStr">
+        <is>
+          <t>19:37:23</t>
+        </is>
+      </c>
+      <c r="C126" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SRM</t>
+        </is>
+      </c>
+      <c r="D126" s="4" t="inlineStr">
+        <is>
+          <t>매도</t>
+        </is>
+      </c>
+      <c r="E126" s="4" t="inlineStr">
+        <is>
+          <t>24.18692821</t>
+        </is>
+      </c>
+      <c r="F126" s="4" t="inlineStr">
+        <is>
+          <t>00121b7b-afd9-4c30-9cea-cc479b73e319</t>
+        </is>
+      </c>
+      <c r="G126" s="4" t="n">
+        <v>4652.89874402</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="4" t="inlineStr">
+        <is>
+          <t>2022-04-02</t>
+        </is>
+      </c>
+      <c r="B127" s="4" t="inlineStr">
+        <is>
+          <t>19:38:06</t>
+        </is>
+      </c>
+      <c r="C127" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D127" s="4" t="inlineStr">
+        <is>
+          <t>매수</t>
+        </is>
+      </c>
+      <c r="E127" s="4" t="inlineStr">
+        <is>
+          <t>102880.015</t>
+        </is>
+      </c>
+      <c r="F127" s="4" t="inlineStr">
+        <is>
+          <t>fe89a807-f235-40a6-a890-a008fa37d683</t>
+        </is>
+      </c>
+      <c r="G127" s="4" t="n">
+        <v>1033975.51984083</v>
       </c>
     </row>
   </sheetData>
@@ -3676,16 +4796,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
   <cols>
     <col width="11.7109375" bestFit="1" customWidth="1" style="8" min="2" max="3"/>
     <col width="19.140625" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
@@ -5720,25 +6840,297 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
+      <c r="A117" s="4" t="inlineStr">
         <is>
           <t>KRW-SXP</t>
         </is>
       </c>
-      <c r="B117" t="n">
+      <c r="B117" s="4" t="n">
         <v>2130</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117" s="4" t="n">
         <v>2021</v>
       </c>
-      <c r="D117" s="12" t="n">
-        <v>44648.65413270563</v>
-      </c>
-      <c r="E117" t="n">
+      <c r="D117" s="11" t="n">
+        <v>44648.65413270833</v>
+      </c>
+      <c r="E117" s="4" t="n">
         <v>101251.2</v>
       </c>
-      <c r="F117" t="n">
+      <c r="F117" s="4" t="n">
         <v>1017606.7580248</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B118" s="11" t="n">
+        <v>44649.83895396991</v>
+      </c>
+      <c r="C118" s="4" t="n">
+        <v>100534.8</v>
+      </c>
+      <c r="D118" s="4" t="n">
+        <v>1010409.2032066</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B119" s="11" t="n">
+        <v>44649.84219458333</v>
+      </c>
+      <c r="C119" s="4" t="n">
+        <v>99973.17</v>
+      </c>
+      <c r="D119" s="4" t="n">
+        <v>1009832.43839433</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B120" s="11" t="n">
+        <v>44649.84495008102</v>
+      </c>
+      <c r="C120" s="4" t="n">
+        <v>100407.44</v>
+      </c>
+      <c r="D120" s="4" t="n">
+        <v>1009127.34035862</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="4" t="inlineStr">
+        <is>
+          <t>KRW-WAVES</t>
+        </is>
+      </c>
+      <c r="B121" s="11" t="n">
+        <v>44650.05405233796</v>
+      </c>
+      <c r="C121" s="4" t="n">
+        <v>100897.975</v>
+      </c>
+      <c r="D121" s="4" t="n">
+        <v>1014058.79312318</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4" t="inlineStr">
+        <is>
+          <t>KRW-BTC</t>
+        </is>
+      </c>
+      <c r="B122" s="11" t="n">
+        <v>44650.31980175926</v>
+      </c>
+      <c r="C122" s="4" t="n">
+        <v>101501.94</v>
+      </c>
+      <c r="D122" s="4" t="n">
+        <v>1020128.99385442</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>44653.00335386574</v>
+      </c>
+      <c r="C123" s="4" t="n">
+        <v>101687.01</v>
+      </c>
+      <c r="D123" s="4" t="n">
+        <v>1021988.67862877</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ETH</t>
+        </is>
+      </c>
+      <c r="B124" s="11" t="n">
+        <v>44653.0554040162</v>
+      </c>
+      <c r="C124" s="4" t="n">
+        <v>101783.525</v>
+      </c>
+      <c r="D124" s="4" t="n">
+        <v>1022955.19242762</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SOL</t>
+        </is>
+      </c>
+      <c r="B125" s="11" t="n">
+        <v>44653.1290149074</v>
+      </c>
+      <c r="C125" s="4" t="n">
+        <v>101875.065</v>
+      </c>
+      <c r="D125" s="4" t="n">
+        <v>1023877.07188922</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="4" t="inlineStr">
+        <is>
+          <t>KRW-ZIL</t>
+        </is>
+      </c>
+      <c r="B126" s="11" t="n">
+        <v>44653.38393679398</v>
+      </c>
+      <c r="C126" s="4" t="n">
+        <v>101954.665</v>
+      </c>
+      <c r="D126" s="4" t="n">
+        <v>1024674.92249907</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="4" t="inlineStr">
+        <is>
+          <t>KRW-AXS</t>
+        </is>
+      </c>
+      <c r="B127" s="11" t="n">
+        <v>44653.39849383102</v>
+      </c>
+      <c r="C127" s="4" t="n">
+        <v>102073.07</v>
+      </c>
+      <c r="D127" s="4" t="n">
+        <v>1025869.73019221</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="B128" s="11" t="n">
+        <v>44653.43058582176</v>
+      </c>
+      <c r="C128" s="4" t="n">
+        <v>102280.03</v>
+      </c>
+      <c r="D128" s="4" t="n">
+        <v>1027947.85749579</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="B129" s="11" t="n">
+        <v>44653.71838363426</v>
+      </c>
+      <c r="C129" s="4" t="n">
+        <v>102389.48</v>
+      </c>
+      <c r="D129" s="4" t="n">
+        <v>1029047.59688842</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="B130" s="11" t="n">
+        <v>44653.71928302084</v>
+      </c>
+      <c r="C130" s="4" t="n">
+        <v>102494.95</v>
+      </c>
+      <c r="D130" s="4" t="n">
+        <v>1030109.61267686</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="4" t="inlineStr">
+        <is>
+          <t>KRW-MED</t>
+        </is>
+      </c>
+      <c r="B131" s="11" t="n">
+        <v>44653.72125877315</v>
+      </c>
+      <c r="C131" s="4" t="n">
+        <v>102625.295</v>
+      </c>
+      <c r="D131" s="4" t="n">
+        <v>1031410.4561176</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4" t="inlineStr">
+        <is>
+          <t>KRW-FLOW</t>
+        </is>
+      </c>
+      <c r="B132" s="11" t="n">
+        <v>44653.72521373843</v>
+      </c>
+      <c r="C132" s="4" t="n">
+        <v>102702.905</v>
+      </c>
+      <c r="D132" s="4" t="n">
+        <v>1032193.17962218</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="4" t="inlineStr">
+        <is>
+          <t>KRW-SRM</t>
+        </is>
+      </c>
+      <c r="B133" s="11" t="n">
+        <v>44653.80593075231</v>
+      </c>
+      <c r="C133" s="4" t="n">
+        <v>102794.445</v>
+      </c>
+      <c r="D133" s="4" t="n">
+        <v>1033111.32089588</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="B134" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C134" s="4" t="n">
+        <v>102880.015</v>
+      </c>
+      <c r="D134" s="4" t="n">
+        <v>1033975.51984083</v>
       </c>
     </row>
   </sheetData>
@@ -5752,16 +7144,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
   <cols>
     <col width="37.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="19.140625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -5798,6 +7190,474 @@
       <c r="F1" s="7" t="inlineStr">
         <is>
           <t>매수 / 매도</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>b51e7553-9b00-433a-9353-130e262a6f5f</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>102.880015</v>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>80eff433-5f1a-4df5-b887-4cdb4b2ca120</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>970</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>106.06187113</v>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>55c6329b-7b38-4883-8dec-2041cea0b5f8</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>940</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>109.44682447</v>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>d1f9b64c-c867-4a58-a02b-ce232237a3a5</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>910</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>113.05496154</v>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>aee93e96-c201-49a3-8ef3-aeb8d1c5ab9c</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>880</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>116.90910795</v>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>933ec712-baf2-48e5-b3b5-e8f734233836</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>850</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>121.03531176</v>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>612dd51d-f523-4505-98b8-7c5bfed16924</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>820</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>125.46343293</v>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>2cc2dfce-287c-4680-ac87-ef686c9469fc</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>790</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>130.22786709</v>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>001d1fda-97d2-4505-875b-715e6699bbf4</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>760</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>135.36844079</v>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17d390b5-8eb2-47e8-9583-98153ea7adba</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>102.880015</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>39f4a988-ae04-4336-aa8f-1d9b7a3c3c66</t>
+        </is>
+      </c>
+      <c r="B12" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>970</v>
+      </c>
+      <c r="E12" t="n">
+        <v>106.06187113</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ac08dc6d-59b0-4002-8dd1-4bd75da93e23</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>940</v>
+      </c>
+      <c r="E13" t="n">
+        <v>109.44682447</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>57e2e48f-398d-42ed-9c4e-82fbca63daec</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>910</v>
+      </c>
+      <c r="E14" t="n">
+        <v>113.05496154</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>d18bdce4-694b-4a13-9bba-3ead8563e2db</t>
+        </is>
+      </c>
+      <c r="B15" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>880</v>
+      </c>
+      <c r="E15" t="n">
+        <v>116.90910795</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>29b24350-775e-4f09-999e-47a502ce9728</t>
+        </is>
+      </c>
+      <c r="B16" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>850</v>
+      </c>
+      <c r="E16" t="n">
+        <v>121.03531176</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>7347431e-9b14-41eb-9725-a583a5a593fa</t>
+        </is>
+      </c>
+      <c r="B17" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>820</v>
+      </c>
+      <c r="E17" t="n">
+        <v>125.46343293</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>db9621c6-fd3f-4859-abf4-206f63c55846</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>790</v>
+      </c>
+      <c r="E18" t="n">
+        <v>130.22786709</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>52145c83-2aed-421a-b4ae-85d752b7dfb8</t>
+        </is>
+      </c>
+      <c r="B19" s="12" t="n">
+        <v>44653.86655512063</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>KRW-XRP</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>760</v>
+      </c>
+      <c r="E19" t="n">
+        <v>135.36844079</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>거미줄매수</t>
         </is>
       </c>
     </row>
@@ -5812,13 +7672,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" outlineLevelCol="0"/>
   <cols>
     <col width="19.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.7109375" customWidth="1" style="8" min="2" max="2"/>
@@ -5877,11 +7737,207 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="n">
+      <c r="A7" s="11" t="n">
         <v>44648.65413270833</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1017606.7580248</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="n">
+        <v>44649.83629413194</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>1010986.29909927</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="n">
+        <v>44649.83895396991</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>1010409.2032066</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="n">
+        <v>44649.84219458333</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>1009832.43839433</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="n">
+        <v>44649.84495008102</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>1009127.34035862</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n">
+        <v>44650.05405233796</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>1014058.79312318</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="n">
+        <v>44650.31980175926</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>1020128.99385442</v>
+      </c>
+      <c r="C13" s="4">
+        <f>B13-B12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="n">
+        <v>44653.00335386574</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>1021988.67862877</v>
+      </c>
+      <c r="C14" s="4">
+        <f>B14-B13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="n">
+        <v>44653.0554040162</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>1022955.19242762</v>
+      </c>
+      <c r="C15" s="4">
+        <f>B15-B14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n">
+        <v>44653.1290149074</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>1023877.07188922</v>
+      </c>
+      <c r="C16" s="4">
+        <f>B16-B15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="n">
+        <v>44653.38393679398</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>1024674.92249907</v>
+      </c>
+      <c r="C17" s="4">
+        <f>B17-B16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="n">
+        <v>44653.39849383102</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>1025869.73019221</v>
+      </c>
+      <c r="C18" s="4">
+        <f>B18-B17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="n">
+        <v>44653.43058582176</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>1027947.85749579</v>
+      </c>
+      <c r="C19" s="4">
+        <f>B19-B18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="n">
+        <v>44653.71838363426</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>1029047.59688842</v>
+      </c>
+      <c r="C20" s="4">
+        <f>B20-B19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="n">
+        <v>44653.71928302084</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>1030109.61267686</v>
+      </c>
+      <c r="C21" s="4">
+        <f>B21-B20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="n">
+        <v>44653.72125877315</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>1031410.4561176</v>
+      </c>
+      <c r="C22" s="4">
+        <f>B22-B21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="n">
+        <v>44653.72521373843</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>1032193.17962218</v>
+      </c>
+      <c r="C23" s="4">
+        <f>B23-B22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="n">
+        <v>44653.80593075231</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>1033111.32089588</v>
+      </c>
+      <c r="C24" s="4">
+        <f>B24-B23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="n">
+        <v>44653.81812458333</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>1033975.51984083</v>
+      </c>
+      <c r="C25" s="4">
+        <f>B25-B24</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>